<commit_message>
nate making his first plot
</commit_message>
<xml_diff>
--- a/raw_ts_data/fd/fd12_metadata.xlsx
+++ b/raw_ts_data/fd/fd12_metadata.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ncw02\Downloads\IGEA\raw_ts_data\fd\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF9A731B-4E5E-4247-8F11-6563718B9005}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0995EC1-C1B6-4383-9C40-CD9946B0CDA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{02675917-6FB0-1F44-8417-5533CB1D953F}"/>
   </bookViews>
@@ -305,7 +305,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -327,6 +327,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -352,7 +358,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -368,13 +374,15 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="1" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -695,7 +703,7 @@
   <dimension ref="A1:AB999"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+      <selection activeCell="J2" sqref="J2:L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.21875" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -714,65 +722,65 @@
     <col min="15" max="15" width="57.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" s="13" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="11"/>
-      <c r="B1" s="11" t="s">
+    <row r="1" spans="1:28" s="11" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="9"/>
+      <c r="B1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="D1" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="E1" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="F1" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="11" t="s">
+      <c r="G1" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="11" t="s">
+      <c r="H1" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="11" t="s">
+      <c r="I1" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="11" t="s">
+      <c r="J1" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="11" t="s">
+      <c r="K1" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="11" t="s">
+      <c r="L1" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="11" t="s">
+      <c r="M1" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="11" t="s">
+      <c r="N1" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="O1" s="11" t="s">
+      <c r="O1" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="P1" s="11" t="s">
+      <c r="P1" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="Q1" s="11"/>
-      <c r="R1" s="11"/>
-      <c r="S1" s="11"/>
-      <c r="T1" s="11"/>
-      <c r="U1" s="11"/>
-      <c r="V1" s="11"/>
-      <c r="W1" s="11"/>
-      <c r="X1" s="11"/>
-      <c r="Y1" s="11"/>
-      <c r="Z1" s="11"/>
-      <c r="AA1" s="11"/>
-      <c r="AB1" s="11"/>
+      <c r="Q1" s="9"/>
+      <c r="R1" s="9"/>
+      <c r="S1" s="9"/>
+      <c r="T1" s="9"/>
+      <c r="U1" s="9"/>
+      <c r="V1" s="9"/>
+      <c r="W1" s="9"/>
+      <c r="X1" s="9"/>
+      <c r="Y1" s="9"/>
+      <c r="Z1" s="9"/>
+      <c r="AA1" s="9"/>
+      <c r="AB1" s="9"/>
     </row>
     <row r="2" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">
@@ -796,13 +804,19 @@
       <c r="H2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="I2" s="9" t="s">
+      <c r="I2" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="J2" s="10"/>
-      <c r="K2" s="10"/>
-      <c r="L2" s="10"/>
-      <c r="M2" s="10"/>
+      <c r="J2" s="17">
+        <v>423111</v>
+      </c>
+      <c r="K2" s="17">
+        <v>7628839</v>
+      </c>
+      <c r="L2" s="17">
+        <v>513</v>
+      </c>
+      <c r="M2" s="16"/>
       <c r="N2" s="1" t="s">
         <v>18</v>
       </c>
@@ -964,6 +978,15 @@
       <c r="I6" s="1" t="s">
         <v>29</v>
       </c>
+      <c r="J6" s="14">
+        <v>420493</v>
+      </c>
+      <c r="K6" s="14">
+        <v>7622832</v>
+      </c>
+      <c r="L6" s="14">
+        <v>589</v>
+      </c>
       <c r="O6" s="5" t="s">
         <v>30</v>
       </c>
@@ -1586,19 +1609,19 @@
       </c>
     </row>
     <row r="23" spans="2:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="15" t="s">
+      <c r="B23" s="13" t="s">
         <v>72</v>
       </c>
       <c r="C23" s="2">
         <v>44711</v>
       </c>
-      <c r="D23" s="14">
+      <c r="D23" s="12">
         <v>0.63055555555555554</v>
       </c>
-      <c r="E23" s="14">
+      <c r="E23" s="12">
         <v>0.77708333333333324</v>
       </c>
-      <c r="F23" s="14">
+      <c r="F23" s="12">
         <v>0.6875</v>
       </c>
       <c r="G23">
@@ -1630,19 +1653,19 @@
       </c>
     </row>
     <row r="24" spans="2:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="15" t="s">
+      <c r="B24" s="13" t="s">
         <v>73</v>
       </c>
       <c r="C24" s="2">
         <v>44712</v>
       </c>
-      <c r="D24" s="14">
+      <c r="D24" s="12">
         <v>0.60416666666666663</v>
       </c>
-      <c r="E24" s="14">
+      <c r="E24" s="12">
         <v>0.77083333333333337</v>
       </c>
-      <c r="F24" s="14">
+      <c r="F24" s="12">
         <v>0.67361111111111116</v>
       </c>
       <c r="G24">
@@ -4599,9 +4622,6 @@
       <c r="C999" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="I2:M2"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>